<commit_message>
Finished Excel tests :)
</commit_message>
<xml_diff>
--- a/wdio-tests/test/urls.xlsx
+++ b/wdio-tests/test/urls.xlsx
@@ -397,7 +397,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B15"/>
+  <dimension ref="A1:C15"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -407,6 +407,9 @@
         <v>Index</v>
       </c>
       <c r="B1" t="str">
+        <v>Title</v>
+      </c>
+      <c r="C1" t="str">
         <v>Link</v>
       </c>
     </row>
@@ -415,6 +418,9 @@
         <v>1</v>
       </c>
       <c r="B2" t="str">
+        <v>X-COM - Wikipedia, la enciclopedia libre</v>
+      </c>
+      <c r="C2" t="str">
         <v>https://es.wikipedia.org/wiki/X-COM</v>
       </c>
     </row>
@@ -423,6 +429,9 @@
         <v>2</v>
       </c>
       <c r="B3" t="str">
+        <v>Ahorra un 80 % en XCOM: Enemy Unknown en Steam</v>
+      </c>
+      <c r="C3" t="str">
         <v>https://store.steampowered.com/app/200510/XCOM_Enemy_Unknown/?l=spanish</v>
       </c>
     </row>
@@ -431,6 +440,9 @@
         <v>3</v>
       </c>
       <c r="B4" t="str">
+        <v>XCOM 2</v>
+      </c>
+      <c r="C4" t="str">
         <v>https://xcom.com/</v>
       </c>
     </row>
@@ -439,6 +451,9 @@
         <v>4</v>
       </c>
       <c r="B5" t="str">
+        <v>No Title</v>
+      </c>
+      <c r="C5" t="str">
         <v>https://es.wikipedia.org/wiki/XCOM_2</v>
       </c>
     </row>
@@ -447,6 +462,9 @@
         <v>5</v>
       </c>
       <c r="B6" t="str">
+        <v>No Title</v>
+      </c>
+      <c r="C6" t="str">
         <v>https://vandal.elespanol.com/sagas/xcom</v>
       </c>
     </row>
@@ -455,6 +473,9 @@
         <v>6</v>
       </c>
       <c r="B7" t="str">
+        <v>No Title</v>
+      </c>
+      <c r="C7" t="str">
         <v>https://translate.google.com/translate?u=https://www.turtlebeach.com/blog/xcom-3-release&amp;hl=es&amp;sl=en&amp;tl=es&amp;client=rq&amp;prev=search</v>
       </c>
     </row>
@@ -463,6 +484,9 @@
         <v>7</v>
       </c>
       <c r="B8" t="str">
+        <v>No Title</v>
+      </c>
+      <c r="C8" t="str">
         <v>https://www.turtlebeach.com/blog/xcom-3-release</v>
       </c>
     </row>
@@ -471,6 +495,9 @@
         <v>8</v>
       </c>
       <c r="B9" t="str">
+        <v>No Title</v>
+      </c>
+      <c r="C9" t="str">
         <v>https://www.reddit.com/r/Xcom/comments/168a05h/what_is_xcom/?tl=es-es</v>
       </c>
     </row>
@@ -479,6 +506,9 @@
         <v>9</v>
       </c>
       <c r="B10" t="str">
+        <v>Comprar XCOM®: Enemy Unknown</v>
+      </c>
+      <c r="C10" t="str">
         <v>https://www.xbox.com/es-AR/games/store/xcom-enemy-unknown/BQZ0V5R1HPXF</v>
       </c>
     </row>
@@ -487,6 +517,9 @@
         <v>10</v>
       </c>
       <c r="B11" t="str">
+        <v>XCOM 2 Collection - Apps en Google Play</v>
+      </c>
+      <c r="C11" t="str">
         <v>https://play.google.com/store/apps/details?id=com.feralinteractive.xcom2_android&amp;hl=es_AR</v>
       </c>
     </row>
@@ -495,6 +528,9 @@
         <v>11</v>
       </c>
       <c r="B12" t="str">
+        <v>Xcom Ps3 | MercadoLibre</v>
+      </c>
+      <c r="C12" t="str">
         <v>https://listado.mercadolibre.com.ar/xcom-ps3</v>
       </c>
     </row>
@@ -503,6 +539,9 @@
         <v>12</v>
       </c>
       <c r="B13" t="str">
+        <v>Xcom</v>
+      </c>
+      <c r="C13" t="str">
         <v>https://twitter.com/xcom</v>
       </c>
     </row>
@@ -511,6 +550,9 @@
         <v>13</v>
       </c>
       <c r="B14" t="str">
+        <v>Todos los juegos de XCOM - Saga completa</v>
+      </c>
+      <c r="C14" t="str">
         <v>https://vandal.elespanol.com/sagas/xcom</v>
       </c>
     </row>
@@ -519,12 +561,15 @@
         <v>14</v>
       </c>
       <c r="B15" t="str">
-        <v>https://store.2k.com/es/game/buy-xcom-2-pc?srsltid=AfmBOooDTfjrd7Qoc-1cisq0J08W0Vu7ISLnSgleM6EtkWf08QSB3x83</v>
+        <v>XCOM 2</v>
+      </c>
+      <c r="C15" t="str">
+        <v>https://store.2k.com/es/game/buy-xcom-2-pc?srsltid=AfmBOoqcvQrXcFeuNrafqptyWYzHAs-rjukDGJTw5LRqoiLUbuywdmj7</v>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:B15"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:C15"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>